<commit_message>
datawork for process 3
</commit_message>
<xml_diff>
--- a/given.xlsx
+++ b/given.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\11-Chat GPT(wine)\project\data-prepare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\11-wineservice(chatgpt)\project\data-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E719FE1-5627-4E7E-88BD-D38134025217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C74B6D5-74BD-433F-8670-98706DA29FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3890" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4026" uniqueCount="749">
   <si>
     <t>shop_code</t>
   </si>
@@ -2431,12 +2431,18 @@
       <t xml:space="preserve"> priority descriptor</t>
     </r>
   </si>
+  <si>
+    <t>product_url</t>
+  </si>
+  <si>
+    <t>https://www.example.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2584,6 +2590,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2886,7 +2900,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2929,8 +2943,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2938,8 +2953,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2973,6 +2989,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -3293,15 +3310,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT136"/>
+  <dimension ref="A1:AU136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AU1" sqref="AU1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.77734375" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.44140625" customWidth="1"/>
+    <col min="17" max="17" width="98.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="0" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="0" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="0" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.77734375" hidden="1" customWidth="1"/>
+    <col min="34" max="39" width="0" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="141.109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="30.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3440,8 +3484,11 @@
       <c r="AT1" t="s">
         <v>45</v>
       </c>
+      <c r="AU1" t="s">
+        <v>747</v>
+      </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -3568,8 +3615,11 @@
       <c r="AS2">
         <v>1</v>
       </c>
+      <c r="AU2" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -3696,8 +3746,11 @@
       <c r="AT3" t="s">
         <v>90</v>
       </c>
+      <c r="AU3" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -3821,8 +3874,11 @@
       <c r="AS4">
         <v>0</v>
       </c>
+      <c r="AU4" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -3952,8 +4008,11 @@
       <c r="AS5">
         <v>0</v>
       </c>
+      <c r="AU5" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -4086,8 +4145,11 @@
       <c r="AS6">
         <v>1</v>
       </c>
+      <c r="AU6" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -4220,8 +4282,11 @@
       <c r="AS7">
         <v>0</v>
       </c>
+      <c r="AU7" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -4351,8 +4416,11 @@
       <c r="AS8">
         <v>0</v>
       </c>
+      <c r="AU8" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -4482,8 +4550,11 @@
       <c r="AS9">
         <v>0</v>
       </c>
+      <c r="AU9" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -4610,8 +4681,11 @@
       <c r="AS10">
         <v>1</v>
       </c>
+      <c r="AU10" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -4744,8 +4818,11 @@
       <c r="AS11">
         <v>0</v>
       </c>
+      <c r="AU11" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -4872,8 +4949,11 @@
       <c r="AT12" t="s">
         <v>210</v>
       </c>
+      <c r="AU12" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -5003,8 +5083,11 @@
       <c r="AS13">
         <v>0</v>
       </c>
+      <c r="AU13" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -5131,8 +5214,11 @@
       <c r="AS14">
         <v>1</v>
       </c>
+      <c r="AU14" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -5262,8 +5348,11 @@
       <c r="AS15">
         <v>1</v>
       </c>
+      <c r="AU15" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -5390,8 +5479,11 @@
       <c r="AT16" t="s">
         <v>210</v>
       </c>
+      <c r="AU16" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -5515,8 +5607,11 @@
       <c r="AS17">
         <v>0</v>
       </c>
+      <c r="AU17" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -5643,8 +5738,11 @@
       <c r="AT18" t="s">
         <v>245</v>
       </c>
+      <c r="AU18" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -5771,8 +5869,11 @@
       <c r="AS19">
         <v>1</v>
       </c>
+      <c r="AU19" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -5905,8 +6006,11 @@
       <c r="AS20">
         <v>0</v>
       </c>
+      <c r="AU20" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -6033,8 +6137,11 @@
       <c r="AS21">
         <v>0</v>
       </c>
+      <c r="AU21" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -6161,8 +6268,11 @@
       <c r="AS22">
         <v>0</v>
       </c>
+      <c r="AU22" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -6292,8 +6402,11 @@
       <c r="AS23">
         <v>0</v>
       </c>
+      <c r="AU23" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -6423,8 +6536,11 @@
       <c r="AT24" t="s">
         <v>314</v>
       </c>
+      <c r="AU24" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -6551,8 +6667,11 @@
       <c r="AS25">
         <v>0</v>
       </c>
+      <c r="AU25" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -6685,8 +6804,11 @@
       <c r="AT26" t="s">
         <v>327</v>
       </c>
+      <c r="AU26" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -6819,8 +6941,11 @@
       <c r="AS27">
         <v>1</v>
       </c>
+      <c r="AU27" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -6947,8 +7072,11 @@
       <c r="AS28">
         <v>1</v>
       </c>
+      <c r="AU28" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -7078,8 +7206,11 @@
       <c r="AS29">
         <v>1</v>
       </c>
+      <c r="AU29" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -7209,8 +7340,11 @@
       <c r="AS30">
         <v>1</v>
       </c>
+      <c r="AU30" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -7343,8 +7477,11 @@
       <c r="AS31">
         <v>1</v>
       </c>
+      <c r="AU31" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -7474,8 +7611,11 @@
       <c r="AS32">
         <v>1</v>
       </c>
+      <c r="AU32" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -7605,8 +7745,11 @@
       <c r="AT33" t="s">
         <v>354</v>
       </c>
+      <c r="AU33" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -7733,8 +7876,11 @@
       <c r="AT34" t="s">
         <v>359</v>
       </c>
+      <c r="AU34" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -7864,8 +8010,11 @@
       <c r="AS35">
         <v>0</v>
       </c>
+      <c r="AU35" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -7998,8 +8147,11 @@
       <c r="AS36">
         <v>0</v>
       </c>
+      <c r="AU36" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -8135,8 +8287,11 @@
       <c r="AT37" t="s">
         <v>382</v>
       </c>
+      <c r="AU37" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -8266,8 +8421,11 @@
       <c r="AS38">
         <v>0</v>
       </c>
+      <c r="AU38" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -8400,8 +8558,11 @@
       <c r="AS39">
         <v>0</v>
       </c>
+      <c r="AU39" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -8534,8 +8695,11 @@
       <c r="AT40" t="s">
         <v>327</v>
       </c>
+      <c r="AU40" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -8662,8 +8826,11 @@
       <c r="AS41">
         <v>0</v>
       </c>
+      <c r="AU41" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -8796,8 +8963,11 @@
       <c r="AS42">
         <v>1</v>
       </c>
+      <c r="AU42" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -8921,8 +9091,11 @@
       <c r="AS43">
         <v>0</v>
       </c>
+      <c r="AU43" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -9052,8 +9225,11 @@
       <c r="AS44">
         <v>1</v>
       </c>
+      <c r="AU44" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -9180,8 +9356,11 @@
       <c r="AT45" t="s">
         <v>314</v>
       </c>
+      <c r="AU45" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -9314,8 +9493,11 @@
       <c r="AS46">
         <v>1</v>
       </c>
+      <c r="AU46" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -9445,8 +9627,11 @@
       <c r="AS47">
         <v>0</v>
       </c>
+      <c r="AU47" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -9573,8 +9758,11 @@
       <c r="AS48">
         <v>0</v>
       </c>
+      <c r="AU48" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="49" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -9704,8 +9892,11 @@
       <c r="AS49">
         <v>1</v>
       </c>
+      <c r="AU49" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="50" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -9832,8 +10023,11 @@
       <c r="AT50" t="s">
         <v>210</v>
       </c>
+      <c r="AU50" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="51" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>46</v>
       </c>
@@ -9960,8 +10154,11 @@
       <c r="AT51" t="s">
         <v>210</v>
       </c>
+      <c r="AU51" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="52" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -10088,8 +10285,11 @@
       <c r="AS52">
         <v>1</v>
       </c>
+      <c r="AU52" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="53" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -10216,8 +10416,11 @@
       <c r="AS53">
         <v>1</v>
       </c>
+      <c r="AU53" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="54" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -10344,8 +10547,11 @@
       <c r="AS54">
         <v>1</v>
       </c>
+      <c r="AU54" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="55" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>46</v>
       </c>
@@ -10472,8 +10678,11 @@
       <c r="AS55">
         <v>0</v>
       </c>
+      <c r="AU55" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="56" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>46</v>
       </c>
@@ -10606,8 +10815,11 @@
       <c r="AS56">
         <v>0</v>
       </c>
+      <c r="AU56" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="57" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>46</v>
       </c>
@@ -10737,8 +10949,11 @@
       <c r="AT57" t="s">
         <v>459</v>
       </c>
+      <c r="AU57" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="58" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>46</v>
       </c>
@@ -10865,8 +11080,11 @@
       <c r="AS58">
         <v>0</v>
       </c>
+      <c r="AU58" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="59" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>46</v>
       </c>
@@ -10993,8 +11211,11 @@
       <c r="AS59">
         <v>1</v>
       </c>
+      <c r="AU59" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="60" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>46</v>
       </c>
@@ -11121,8 +11342,11 @@
       <c r="AS60">
         <v>1</v>
       </c>
+      <c r="AU60" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="61" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>46</v>
       </c>
@@ -11249,8 +11473,11 @@
       <c r="AS61">
         <v>1</v>
       </c>
+      <c r="AU61" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="62" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>46</v>
       </c>
@@ -11377,8 +11604,11 @@
       <c r="AT62" t="s">
         <v>210</v>
       </c>
+      <c r="AU62" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="63" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>46</v>
       </c>
@@ -11508,8 +11738,11 @@
       <c r="AT63" t="s">
         <v>327</v>
       </c>
+      <c r="AU63" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="64" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>46</v>
       </c>
@@ -11636,8 +11869,11 @@
       <c r="AS64">
         <v>0</v>
       </c>
+      <c r="AU64" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="65" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>46</v>
       </c>
@@ -11761,8 +11997,11 @@
       <c r="AS65">
         <v>0</v>
       </c>
+      <c r="AU65" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="66" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>46</v>
       </c>
@@ -11895,8 +12134,11 @@
       <c r="AS66">
         <v>1</v>
       </c>
+      <c r="AU66" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="67" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>46</v>
       </c>
@@ -12026,8 +12268,11 @@
       <c r="AS67">
         <v>1</v>
       </c>
+      <c r="AU67" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="68" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>46</v>
       </c>
@@ -12157,8 +12402,11 @@
       <c r="AS68">
         <v>1</v>
       </c>
+      <c r="AU68" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="69" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>46</v>
       </c>
@@ -12288,8 +12536,11 @@
       <c r="AS69">
         <v>0</v>
       </c>
+      <c r="AU69" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="70" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>46</v>
       </c>
@@ -12419,8 +12670,11 @@
       <c r="AS70">
         <v>0</v>
       </c>
+      <c r="AU70" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="71" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>46</v>
       </c>
@@ -12550,8 +12804,11 @@
       <c r="AS71">
         <v>1</v>
       </c>
+      <c r="AU71" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="72" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>46</v>
       </c>
@@ -12681,8 +12938,11 @@
       <c r="AS72">
         <v>0</v>
       </c>
+      <c r="AU72" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="73" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>46</v>
       </c>
@@ -12809,8 +13069,11 @@
       <c r="AS73">
         <v>1</v>
       </c>
+      <c r="AU73" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="74" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>46</v>
       </c>
@@ -12937,8 +13200,11 @@
       <c r="AS74">
         <v>1</v>
       </c>
+      <c r="AU74" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="75" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>46</v>
       </c>
@@ -13068,8 +13334,11 @@
       <c r="AS75">
         <v>0</v>
       </c>
+      <c r="AU75" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="76" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>46</v>
       </c>
@@ -13196,8 +13465,11 @@
       <c r="AS76">
         <v>0</v>
       </c>
+      <c r="AU76" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="77" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>46</v>
       </c>
@@ -13330,8 +13602,11 @@
       <c r="AT77" t="s">
         <v>327</v>
       </c>
+      <c r="AU77" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="78" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>46</v>
       </c>
@@ -13461,8 +13736,11 @@
       <c r="AS78">
         <v>1</v>
       </c>
+      <c r="AU78" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="79" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>46</v>
       </c>
@@ -13595,8 +13873,11 @@
       <c r="AS79">
         <v>1</v>
       </c>
+      <c r="AU79" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="80" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>46</v>
       </c>
@@ -13729,8 +14010,11 @@
       <c r="AT80" t="s">
         <v>354</v>
       </c>
+      <c r="AU80" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="81" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>46</v>
       </c>
@@ -13863,8 +14147,11 @@
       <c r="AS81">
         <v>1</v>
       </c>
+      <c r="AU81" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="82" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>46</v>
       </c>
@@ -13991,8 +14278,11 @@
       <c r="AS82">
         <v>1</v>
       </c>
+      <c r="AU82" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="83" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>46</v>
       </c>
@@ -14122,8 +14412,11 @@
       <c r="AS83">
         <v>1</v>
       </c>
+      <c r="AU83" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="84" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>46</v>
       </c>
@@ -14256,8 +14549,11 @@
       <c r="AS84">
         <v>1</v>
       </c>
+      <c r="AU84" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="85" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>46</v>
       </c>
@@ -14381,8 +14677,11 @@
       <c r="AS85">
         <v>0</v>
       </c>
+      <c r="AU85" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="86" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>46</v>
       </c>
@@ -14512,8 +14811,11 @@
       <c r="AS86">
         <v>0</v>
       </c>
+      <c r="AU86" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="87" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>46</v>
       </c>
@@ -14637,8 +14939,11 @@
       <c r="AS87">
         <v>1</v>
       </c>
+      <c r="AU87" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="88" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>46</v>
       </c>
@@ -14765,8 +15070,11 @@
       <c r="AS88">
         <v>0</v>
       </c>
+      <c r="AU88" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="89" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>46</v>
       </c>
@@ -14893,8 +15201,11 @@
       <c r="AS89">
         <v>1</v>
       </c>
+      <c r="AU89" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="90" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>46</v>
       </c>
@@ -15027,8 +15338,11 @@
       <c r="AS90">
         <v>0</v>
       </c>
+      <c r="AU90" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="91" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>46</v>
       </c>
@@ -15155,8 +15469,11 @@
       <c r="AS91">
         <v>1</v>
       </c>
+      <c r="AU91" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="92" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>46</v>
       </c>
@@ -15289,8 +15606,11 @@
       <c r="AS92">
         <v>1</v>
       </c>
+      <c r="AU92" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="93" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>46</v>
       </c>
@@ -15420,8 +15740,11 @@
       <c r="AS93">
         <v>1</v>
       </c>
+      <c r="AU93" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="94" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>46</v>
       </c>
@@ -15554,8 +15877,11 @@
       <c r="AS94">
         <v>1</v>
       </c>
+      <c r="AU94" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="95" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>46</v>
       </c>
@@ -15685,8 +16011,11 @@
       <c r="AS95">
         <v>0</v>
       </c>
+      <c r="AU95" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="96" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>46</v>
       </c>
@@ -15816,8 +16145,11 @@
       <c r="AS96">
         <v>0</v>
       </c>
+      <c r="AU96" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="97" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>46</v>
       </c>
@@ -15944,8 +16276,11 @@
       <c r="AS97">
         <v>1</v>
       </c>
+      <c r="AU97" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="98" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>46</v>
       </c>
@@ -16072,8 +16407,11 @@
       <c r="AT98" t="s">
         <v>459</v>
       </c>
+      <c r="AU98" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="99" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>46</v>
       </c>
@@ -16203,8 +16541,11 @@
       <c r="AS99">
         <v>1</v>
       </c>
+      <c r="AU99" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="100" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>46</v>
       </c>
@@ -16331,8 +16672,11 @@
       <c r="AS100">
         <v>0</v>
       </c>
+      <c r="AU100" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="101" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>46</v>
       </c>
@@ -16465,8 +16809,11 @@
       <c r="AS101">
         <v>1</v>
       </c>
+      <c r="AU101" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="102" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>46</v>
       </c>
@@ -16596,8 +16943,11 @@
       <c r="AS102">
         <v>0</v>
       </c>
+      <c r="AU102" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="103" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>46</v>
       </c>
@@ -16727,8 +17077,11 @@
       <c r="AS103">
         <v>0</v>
       </c>
+      <c r="AU103" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="104" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>46</v>
       </c>
@@ -16861,8 +17214,11 @@
       <c r="AT104" t="s">
         <v>314</v>
       </c>
+      <c r="AU104" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="105" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>46</v>
       </c>
@@ -16992,8 +17348,11 @@
       <c r="AT105" t="s">
         <v>314</v>
       </c>
+      <c r="AU105" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="106" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>46</v>
       </c>
@@ -17123,8 +17482,11 @@
       <c r="AS106">
         <v>0</v>
       </c>
+      <c r="AU106" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="107" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>46</v>
       </c>
@@ -17251,8 +17613,11 @@
       <c r="AS107">
         <v>1</v>
       </c>
+      <c r="AU107" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="108" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>46</v>
       </c>
@@ -17382,8 +17747,11 @@
       <c r="AS108">
         <v>1</v>
       </c>
+      <c r="AU108" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="109" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>46</v>
       </c>
@@ -17513,8 +17881,11 @@
       <c r="AS109">
         <v>0</v>
       </c>
+      <c r="AU109" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="110" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>46</v>
       </c>
@@ -17644,8 +18015,11 @@
       <c r="AS110">
         <v>0</v>
       </c>
+      <c r="AU110" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="111" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>46</v>
       </c>
@@ -17775,8 +18149,11 @@
       <c r="AT111" t="s">
         <v>210</v>
       </c>
+      <c r="AU111" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="112" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>46</v>
       </c>
@@ -17903,8 +18280,11 @@
       <c r="AS112">
         <v>1</v>
       </c>
+      <c r="AU112" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="113" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>46</v>
       </c>
@@ -18034,8 +18414,11 @@
       <c r="AS113">
         <v>0</v>
       </c>
+      <c r="AU113" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="114" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>46</v>
       </c>
@@ -18162,8 +18545,11 @@
       <c r="AS114">
         <v>0</v>
       </c>
+      <c r="AU114" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="115" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>46</v>
       </c>
@@ -18293,8 +18679,11 @@
       <c r="AS115">
         <v>0</v>
       </c>
+      <c r="AU115" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="116" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>46</v>
       </c>
@@ -18421,8 +18810,11 @@
       <c r="AS116">
         <v>0</v>
       </c>
+      <c r="AU116" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="117" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>46</v>
       </c>
@@ -18552,8 +18944,11 @@
       <c r="AS117">
         <v>1</v>
       </c>
+      <c r="AU117" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="118" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>46</v>
       </c>
@@ -18683,8 +19078,11 @@
       <c r="AS118">
         <v>0</v>
       </c>
+      <c r="AU118" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="119" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>46</v>
       </c>
@@ -18811,8 +19209,11 @@
       <c r="AT119" t="s">
         <v>359</v>
       </c>
+      <c r="AU119" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="120" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>46</v>
       </c>
@@ -18942,8 +19343,11 @@
       <c r="AS120">
         <v>1</v>
       </c>
+      <c r="AU120" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="121" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>46</v>
       </c>
@@ -19070,8 +19474,11 @@
       <c r="AT121" t="s">
         <v>459</v>
       </c>
+      <c r="AU121" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="122" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>46</v>
       </c>
@@ -19195,8 +19602,11 @@
       <c r="AS122">
         <v>0</v>
       </c>
+      <c r="AU122" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="123" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>46</v>
       </c>
@@ -19326,8 +19736,11 @@
       <c r="AS123">
         <v>0</v>
       </c>
+      <c r="AU123" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="124" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>46</v>
       </c>
@@ -19460,8 +19873,11 @@
       <c r="AS124">
         <v>0</v>
       </c>
+      <c r="AU124" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="125" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>46</v>
       </c>
@@ -19594,8 +20010,11 @@
       <c r="AS125">
         <v>0</v>
       </c>
+      <c r="AU125" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="126" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>46</v>
       </c>
@@ -19722,8 +20141,11 @@
       <c r="AS126">
         <v>0</v>
       </c>
+      <c r="AU126" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="127" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>46</v>
       </c>
@@ -19850,8 +20272,11 @@
       <c r="AS127">
         <v>1</v>
       </c>
+      <c r="AU127" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="128" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>46</v>
       </c>
@@ -19978,8 +20403,11 @@
       <c r="AS128">
         <v>1</v>
       </c>
+      <c r="AU128" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="129" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>46</v>
       </c>
@@ -20106,8 +20534,11 @@
       <c r="AS129">
         <v>1</v>
       </c>
+      <c r="AU129" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="130" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>46</v>
       </c>
@@ -20237,8 +20668,11 @@
       <c r="AS130">
         <v>0</v>
       </c>
+      <c r="AU130" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="131" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>46</v>
       </c>
@@ -20365,8 +20799,11 @@
       <c r="AS131">
         <v>1</v>
       </c>
+      <c r="AU131" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="132" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>46</v>
       </c>
@@ -20493,8 +20930,11 @@
       <c r="AS132">
         <v>0</v>
       </c>
+      <c r="AU132" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="133" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>46</v>
       </c>
@@ -20624,8 +21064,11 @@
       <c r="AS133">
         <v>1</v>
       </c>
+      <c r="AU133" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="134" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>46</v>
       </c>
@@ -20752,8 +21195,11 @@
       <c r="AS134">
         <v>1</v>
       </c>
+      <c r="AU134" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="135" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>46</v>
       </c>
@@ -20880,8 +21326,11 @@
       <c r="AS135">
         <v>0</v>
       </c>
+      <c r="AU135" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="136" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>46</v>
       </c>
@@ -21011,8 +21460,15 @@
       <c r="AT136" t="s">
         <v>314</v>
       </c>
+      <c r="AU136" s="5" t="s">
+        <v>748</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AU2" r:id="rId1" xr:uid="{81B21EC4-ABA1-483B-AE6C-EF51E793DFED}"/>
+    <hyperlink ref="AU3:AU136" r:id="rId2" display="https://www.example.com" xr:uid="{93666343-5103-4EBA-B39E-445D33BFBAA0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -21021,16 +21477,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>714</v>
       </c>
@@ -21038,7 +21494,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -21046,7 +21502,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -21054,7 +21510,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -21062,7 +21518,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -21070,7 +21526,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -21078,7 +21534,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -21086,7 +21542,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -21094,7 +21550,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -21102,7 +21558,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -21110,7 +21566,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -21118,7 +21574,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -21126,7 +21582,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -21134,7 +21590,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -21142,7 +21598,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -21150,7 +21606,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -21158,7 +21614,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -21166,7 +21622,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -21174,7 +21630,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -21182,7 +21638,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -21190,7 +21646,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -21198,7 +21654,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -21206,7 +21662,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -21214,7 +21670,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -21222,7 +21678,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -21230,7 +21686,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -21238,7 +21694,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -21246,7 +21702,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -21254,7 +21710,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -21262,7 +21718,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -21270,7 +21726,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -21278,7 +21734,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -21286,7 +21742,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -21294,7 +21750,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -21302,7 +21758,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -21310,7 +21766,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -21318,7 +21774,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -21326,7 +21782,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -21334,7 +21790,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -21342,7 +21798,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -21350,7 +21806,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -21358,7 +21814,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -21366,7 +21822,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -21374,7 +21830,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -21382,7 +21838,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -21390,7 +21846,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -21398,7 +21854,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>

</xml_diff>